<commit_message>
end demo week 2
</commit_message>
<xml_diff>
--- a/src/main/java/ml6002b2022/week2_demo/Attribute Quality Calculator.xlsx
+++ b/src/main/java/ml6002b2022/week2_demo/Attribute Quality Calculator.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42407EF7-AA84-4161-919A-11643395580A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2145B6BE-0FCB-4562-B158-BAEE8D72F057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15405" yWindow="1410" windowWidth="22995" windowHeight="19095" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13320" yWindow="510" windowWidth="20745" windowHeight="18225" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entropy" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="47">
   <si>
     <t>Base Node</t>
   </si>
@@ -78,21 +78,6 @@
     <t>Information Gain</t>
   </si>
   <si>
-    <t>H(A1)=</t>
-  </si>
-  <si>
-    <t>H(X)=</t>
-  </si>
-  <si>
-    <t>H(A2)=</t>
-  </si>
-  <si>
-    <t>H(A3)=</t>
-  </si>
-  <si>
-    <t>gain(X,A)=</t>
-  </si>
-  <si>
     <t>Contingency</t>
   </si>
   <si>
@@ -181,6 +166,15 @@
   </si>
   <si>
     <t>GAIN FROM TIERNEY</t>
+  </si>
+  <si>
+    <t>Entropy per class for node</t>
+  </si>
+  <si>
+    <t>Saka</t>
+  </si>
+  <si>
+    <t>GAIN FROM SAKA</t>
   </si>
 </sst>
 </file>
@@ -1923,10 +1917,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A2:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,699 +1930,682 @@
     <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1">
-        <f>I9</f>
-        <v>1.4387586809150084</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1">
-        <f>I17</f>
-        <v>1.3787834934861756</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1">
-        <f>I35</f>
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1">
-        <f>I44</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="e">
-        <f>D1-C15*G1-C33*I35-C42*K1</f>
-        <v>#VALUE!</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5">
+        <f>C4/$C$4</f>
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f>SUM(D7:D9)</f>
+        <v>20</v>
+      </c>
+      <c r="E5" s="1">
+        <f>SUM(E7:E12)</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C7">
-        <f>C6/$C$6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <f>SUM(D9:D11)</f>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E7" s="1">
-        <f>SUM(E9:E14)</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="1"/>
+        <f>D7/$C$4</f>
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="2">
+        <f>E7</f>
+        <v>0.2</v>
+      </c>
+      <c r="G7">
+        <f>IF(E7&lt;&gt;0,E7*LOG(E7,2),0)</f>
+        <v>-0.46438561897747244</v>
+      </c>
+      <c r="I7">
+        <f>-SUM(G7:G10)</f>
+        <v>1.4387586809150084</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
         <v>5</v>
       </c>
-      <c r="I8" t="s">
-        <v>6</v>
+      <c r="E8" s="1">
+        <f>D8/$C$4</f>
+        <v>0.25</v>
+      </c>
+      <c r="F8" s="2">
+        <f>E8</f>
+        <v>0.25</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G9" si="0">IF(E8&lt;&gt;0,E8*LOG(E8,2),0)</f>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1">
-        <f>D9/$C$6</f>
-        <v>0.2</v>
+        <f>D9/$C$4</f>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F9" s="2">
         <f>E9</f>
-        <v>0.2</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G9">
-        <f>IF(E9&lt;&gt;0,E9*LOG(E9,2),0)</f>
-        <v>-0.46438561897747244</v>
-      </c>
-      <c r="I9">
-        <f>-SUM(G9:G12)</f>
-        <v>1.4387586809150084</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10" s="1">
-        <f>D10/$C$6</f>
-        <v>0.25</v>
-      </c>
-      <c r="F10" s="2">
-        <f>E10</f>
-        <v>0.25</v>
-      </c>
-      <c r="G10">
-        <f t="shared" ref="G10:G12" si="0">IF(E10&lt;&gt;0,E10*LOG(E10,2),0)</f>
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1">
-        <f>D11/$C$6</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F11" s="2">
-        <f>E11</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G11">
         <f t="shared" si="0"/>
         <v>-0.47437306193753581</v>
       </c>
     </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E12" s="1"/>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f>C12/$C$4</f>
+        <v>0.35</v>
+      </c>
+      <c r="D13">
+        <f>SUM(D15:D18)</f>
+        <v>7</v>
+      </c>
+      <c r="E13" s="1">
+        <f>SUM(E15:E18)</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
       </c>
       <c r="F14" s="2"/>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C15">
-        <f>C14/$C$6</f>
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <f>SUM(D17:D20)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1">
-        <f>SUM(E17:E20)</f>
-        <v>1</v>
-      </c>
-      <c r="F15" s="2"/>
+        <f>D15/$D$13</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="F15" s="2">
+        <f>E15</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="G15">
+        <f>IF(E15&lt;&gt;0,E15*LOG(E15,2),0)</f>
+        <v>-0.40105070315108637</v>
+      </c>
+      <c r="I15">
+        <f>-SUM(G15:G18)</f>
+        <v>1.3787834934861756</v>
+      </c>
+      <c r="K15">
+        <f>7/20*1.37878</f>
+        <v>0.48257299999999992</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" t="s">
-        <v>5</v>
-      </c>
-      <c r="I16" t="s">
-        <v>6</v>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" ref="E16:E17" si="1">D16/$D$13</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="F16" s="2">
+        <f>E16</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:G17" si="2">IF(E16&lt;&gt;0,E16*LOG(E16,2),0)</f>
+        <v>-0.51638712058788683</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E17" s="1">
-        <f>D17/$D$15</f>
-        <v>0.14285714285714285</v>
+        <f t="shared" si="1"/>
+        <v>0.5714285714285714</v>
       </c>
       <c r="F17" s="2">
         <f>E17</f>
-        <v>0.14285714285714285</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G17">
-        <f>IF(E17&lt;&gt;0,E17*LOG(E17,2),0)</f>
-        <v>-0.40105070315108637</v>
-      </c>
-      <c r="I17">
-        <f>-SUM(G17:G20)</f>
-        <v>1.3787834934861756</v>
+        <f t="shared" si="2"/>
+        <v>-0.46134566974720242</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1">
-        <f t="shared" ref="E18:E19" si="1">D18/$D$15</f>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="F18" s="2">
-        <f>E18</f>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="G18">
-        <f t="shared" ref="G18:G19" si="2">IF(E18&lt;&gt;0,E18*LOG(E18,2),0)</f>
-        <v>-0.51638712058788683</v>
-      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-      <c r="E19" s="1">
-        <f t="shared" si="1"/>
-        <v>0.5714285714285714</v>
+        <v>13</v>
       </c>
       <c r="F19" s="2"/>
-      <c r="G19">
-        <f t="shared" si="2"/>
-        <v>-0.46134566974720242</v>
-      </c>
-      <c r="K19">
-        <f>7/20*I17+13/20*I24</f>
-        <v>1.4297970665753632</v>
-      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E20" s="1"/>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <f>C19/$C$4</f>
+        <v>0.65</v>
+      </c>
+      <c r="D20">
+        <f>SUM(D22:D25)</f>
+        <v>13</v>
+      </c>
+      <c r="E20" s="1">
+        <f>SUM(E22:E25)</f>
+        <v>1</v>
+      </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21">
-        <v>13</v>
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
       </c>
       <c r="F21" s="2"/>
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C22">
-        <f>C21/$C$6</f>
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <f>SUM(D24:D27)</f>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E22" s="1">
-        <f>SUM(E24:E27)</f>
-        <v>1</v>
-      </c>
-      <c r="F22" s="2"/>
+        <f>D22/$D$20</f>
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="F22" s="2">
+        <f>E22</f>
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="G22">
+        <f>IF(E22&lt;&gt;0,E22*LOG(E22,2),0)</f>
+        <v>-0.48818705017383146</v>
+      </c>
+      <c r="I22">
+        <f>-SUM(G22:G25)</f>
+        <v>1.4572659136233872</v>
+      </c>
+      <c r="K22">
+        <f>13/20*I22</f>
+        <v>0.94722284385520172</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" t="s">
-        <v>5</v>
-      </c>
-      <c r="I23" t="s">
-        <v>6</v>
+      <c r="E23" s="1">
+        <f>D23/$D$20</f>
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="F23" s="2">
+        <f>E23</f>
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="G23">
+        <f>IF(E23&lt;&gt;0,E23*LOG(E23,2),0)</f>
+        <v>-0.48818705017383146</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E24" s="1">
-        <f>D24/$D$22</f>
-        <v>0.23076923076923078</v>
+        <f>D24/$D$20</f>
+        <v>0.53846153846153844</v>
       </c>
       <c r="F24" s="2">
         <f>E24</f>
-        <v>0.23076923076923078</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="G24">
         <f>IF(E24&lt;&gt;0,E24*LOG(E24,2),0)</f>
-        <v>-0.48818705017383146</v>
-      </c>
-      <c r="I24">
-        <f>-SUM(G24:G27)</f>
-        <v>1.4572659136233872</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+        <v>-0.48089181327572439</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>42</v>
       </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
-      <c r="E25" s="1">
-        <f>D25/$D$22</f>
-        <v>0.23076923076923078</v>
-      </c>
-      <c r="F25" s="2">
-        <f>E25</f>
-        <v>0.23076923076923078</v>
-      </c>
-      <c r="G25">
-        <f>IF(E25&lt;&gt;0,E25*LOG(E25,2),0)</f>
-        <v>-0.48818705017383146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
       <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>7</v>
-      </c>
-      <c r="E26" s="1">
-        <f>D26/$D$22</f>
-        <v>0.53846153846153844</v>
-      </c>
-      <c r="F26" s="2">
-        <f>E26</f>
-        <v>0.53846153846153844</v>
-      </c>
-      <c r="G26">
-        <f>IF(E26&lt;&gt;0,E26*LOG(E26,2),0)</f>
-        <v>-0.48089181327572439</v>
+        <f>I7-K15-K22</f>
+        <v>8.9628370598067164E-3</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28">
-        <f>I9-K19</f>
-        <v>8.961614339645152E-3</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>44</v>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <f>C29/$C$4</f>
+        <v>0.35</v>
+      </c>
+      <c r="D30">
+        <f>SUM(D32:D35)</f>
+        <v>7</v>
+      </c>
+      <c r="E30" s="1">
+        <f>SUM(E32:E35)</f>
+        <v>1</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31">
-        <v>7</v>
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>3</v>
       </c>
       <c r="F31" s="2"/>
+      <c r="G31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C32">
-        <f>C31/$C$6</f>
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <f>SUM(D34:D37)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E32" s="1">
-        <f>SUM(E34:E37)</f>
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="F32" s="2"/>
+        <f>D32/$D$13</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="F32" s="2">
+        <f>E32</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G32">
+        <f>IF(E32&lt;&gt;0,E32*LOG(E32,2),0)</f>
+        <v>-0.52388246628704915</v>
+      </c>
+      <c r="I32">
+        <f>-SUM(G32:G35)</f>
+        <v>1.4488156357251847</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E33" t="s">
-        <v>3</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="G33" t="s">
-        <v>5</v>
-      </c>
-      <c r="I33" t="s">
-        <v>6</v>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" ref="E33:E34" si="3">D33/$D$13</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="F33" s="2">
+        <f>E33</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ref="G33:G34" si="4">IF(E33&lt;&gt;0,E33*LOG(E33,2),0)</f>
+        <v>-0.40105070315108637</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E34" s="1">
-        <f>D34/$D$15</f>
-        <v>0.2857142857142857</v>
+        <f t="shared" si="3"/>
+        <v>0.42857142857142855</v>
       </c>
       <c r="F34" s="2">
         <f>E34</f>
-        <v>0.2857142857142857</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="G34">
-        <f>IF(E34&lt;&gt;0,E34*LOG(E34,2),0)</f>
-        <v>-0.51638712058788683</v>
-      </c>
-      <c r="I34">
-        <f>-SUM(G34:G37)</f>
-        <v>1.4413202900260225</v>
+        <f t="shared" si="4"/>
+        <v>-0.52388246628704915</v>
+      </c>
+      <c r="K34">
+        <f>7/20*I32+13/20*I39</f>
+        <v>1.3123712892955246</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" s="1">
-        <f t="shared" ref="E35:E36" si="3">D35/$D$15</f>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="F35" s="2">
-        <f>E35</f>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="G35">
-        <f t="shared" ref="G35:G36" si="4">IF(E35&lt;&gt;0,E35*LOG(E35,2),0)</f>
-        <v>-0.40105070315108637</v>
-      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36">
+        <v>13</v>
+      </c>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <f>C36/$C$4</f>
+        <v>0.65</v>
+      </c>
+      <c r="D37">
+        <f>SUM(D39:D42)</f>
+        <v>13</v>
+      </c>
+      <c r="E37" s="1">
+        <f>SUM(E39:E42)</f>
+        <v>1</v>
+      </c>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="1">
-        <f t="shared" si="3"/>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="F36" s="2"/>
-      <c r="G36">
-        <f t="shared" si="4"/>
-        <v>-0.52388246628704915</v>
-      </c>
-      <c r="K36">
-        <f>7/20*I34+13/20*I41</f>
-        <v>1.3097479183008178</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E37" s="1"/>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38">
-        <v>13</v>
-      </c>
       <c r="F38" s="2"/>
+      <c r="G38" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C39">
-        <f>C38/$C$6</f>
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <f>SUM(D41:D44)</f>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E39" s="1">
-        <f>SUM(E41:E44)</f>
-        <v>1</v>
-      </c>
-      <c r="F39" s="2"/>
+        <f>D39/$D$20</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F39" s="2">
+        <f>E39</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G39">
+        <f>IF(E39&lt;&gt;0,E39*LOG(E39,2),0)</f>
+        <v>-0.28464920908777636</v>
+      </c>
+      <c r="I39">
+        <f>-SUM(G39:G42)</f>
+        <v>1.2389012566026307</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" t="s">
-        <v>2</v>
-      </c>
-      <c r="E40" t="s">
-        <v>3</v>
-      </c>
-      <c r="F40" s="2"/>
-      <c r="G40" t="s">
-        <v>5</v>
-      </c>
-      <c r="I40" t="s">
-        <v>6</v>
+      <c r="B40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40" s="1">
+        <f>D40/$D$20</f>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="F40" s="2">
+        <f>E40</f>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="G40">
+        <f>IF(E40&lt;&gt;0,E40*LOG(E40,2),0)</f>
+        <v>-0.52321222096648989</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E41" s="1">
-        <f>D41/$D$22</f>
-        <v>7.6923076923076927E-2</v>
+        <f>D41/$D$20</f>
+        <v>0.61538461538461542</v>
       </c>
       <c r="F41" s="2">
         <f>E41</f>
-        <v>7.6923076923076927E-2</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="G41">
         <f>IF(E41&lt;&gt;0,E41*LOG(E41,2),0)</f>
-        <v>-0.28464920908777636</v>
-      </c>
-      <c r="I41">
-        <f>-SUM(G41:G44)</f>
-        <v>1.2389012566026307</v>
+        <v>-0.43103982654836442</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42">
-        <v>4</v>
-      </c>
-      <c r="E42" s="1">
-        <f>D42/$D$22</f>
-        <v>0.30769230769230771</v>
-      </c>
-      <c r="F42" s="2">
-        <f>E42</f>
-        <v>0.30769230769230771</v>
-      </c>
-      <c r="G42">
-        <f>IF(E42&lt;&gt;0,E42*LOG(E42,2),0)</f>
-        <v>-0.52321222096648989</v>
-      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43">
-        <v>8</v>
-      </c>
-      <c r="E43" s="1">
-        <f>D43/$D$22</f>
-        <v>0.61538461538461542</v>
-      </c>
-      <c r="F43" s="2">
-        <f>E43</f>
-        <v>0.61538461538461542</v>
-      </c>
-      <c r="G43">
-        <f>IF(E43&lt;&gt;0,E43*LOG(E43,2),0)</f>
-        <v>-0.43103982654836442</v>
-      </c>
+        <f>I7-K34</f>
+        <v>0.12638739161948376</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E44" s="1"/>
@@ -2636,22 +2613,274 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45">
-        <f>I9-K36</f>
-        <v>0.12901076261419053</v>
-      </c>
-      <c r="E45" s="1"/>
+        <v>45</v>
+      </c>
       <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E46" s="1"/>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46">
+        <v>9</v>
+      </c>
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E47" s="1"/>
+      <c r="B47" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47">
+        <f>C46/$C$4</f>
+        <v>0.45</v>
+      </c>
+      <c r="D47">
+        <f>SUM(D49:D52)</f>
+        <v>9</v>
+      </c>
+      <c r="E47" s="1">
+        <f>SUM(E49:E52)</f>
+        <v>1.2857142857142856</v>
+      </c>
       <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>3</v>
+      </c>
+      <c r="F48" s="2"/>
+      <c r="G48" t="s">
+        <v>5</v>
+      </c>
+      <c r="I48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49" s="1">
+        <f>D49/$D$13</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="F49" s="2">
+        <f>E49</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G49">
+        <f>IF(E49&lt;&gt;0,E49*LOG(E49,2),0)</f>
+        <v>-0.52388246628704915</v>
+      </c>
+      <c r="I49">
+        <f>-SUM(G49:G52)</f>
+        <v>1.5716473988611475</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" ref="E50:E51" si="5">D50/$D$13</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="F50" s="2">
+        <f>E50</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G50">
+        <f t="shared" ref="G50:G51" si="6">IF(E50&lt;&gt;0,E50*LOG(E50,2),0)</f>
+        <v>-0.52388246628704915</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="5"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="F51" s="2">
+        <f>E51</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="6"/>
+        <v>-0.52388246628704915</v>
+      </c>
+      <c r="K51">
+        <f>7/20*I49+13/20*I56</f>
+        <v>1.2853184345790023</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E52" s="1"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53">
+        <v>11</v>
+      </c>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54">
+        <f>C53/$C$4</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D54">
+        <f>SUM(D56:D59)</f>
+        <v>11</v>
+      </c>
+      <c r="E54" s="1">
+        <f>SUM(E56:E59)</f>
+        <v>0.84615384615384626</v>
+      </c>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>3</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" t="s">
+        <v>5</v>
+      </c>
+      <c r="I55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" s="1">
+        <f>D56/$D$20</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F56" s="2">
+        <f>E56</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G56">
+        <f>IF(E56&lt;&gt;0,E56*LOG(E56,2),0)</f>
+        <v>-0.28464920908777636</v>
+      </c>
+      <c r="I56">
+        <f>-SUM(G56:G59)</f>
+        <v>1.1311412999655395</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>37</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57" s="1">
+        <f>D57/$D$20</f>
+        <v>0.15384615384615385</v>
+      </c>
+      <c r="F57" s="2">
+        <f>E57</f>
+        <v>0.15384615384615385</v>
+      </c>
+      <c r="G57">
+        <f>IF(E57&lt;&gt;0,E57*LOG(E57,2),0)</f>
+        <v>-0.4154522643293988</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>8</v>
+      </c>
+      <c r="E58" s="1">
+        <f>D58/$D$20</f>
+        <v>0.61538461538461542</v>
+      </c>
+      <c r="F58" s="2">
+        <f>E58</f>
+        <v>0.61538461538461542</v>
+      </c>
+      <c r="G58">
+        <f>IF(E58&lt;&gt;0,E58*LOG(E58,2),0)</f>
+        <v>-0.43103982654836442</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E59" s="1"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>46</v>
+      </c>
+      <c r="C60">
+        <f>I7-K51</f>
+        <v>0.15344024633600606</v>
+      </c>
+      <c r="E60" s="1"/>
+      <c r="F60" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2674,10 +2903,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2699,7 +2928,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <f>D18</f>
@@ -2727,7 +2956,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G4">
         <f>D27</f>
@@ -2760,7 +2989,7 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G5">
         <f>D36</f>
@@ -2793,7 +3022,7 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G6">
         <f>D9</f>
@@ -2829,7 +3058,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G7">
         <f>G6/$K$6</f>
@@ -2863,7 +3092,7 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2878,7 +3107,7 @@
         <v>0.4</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G9">
         <f>G$7*$K3</f>
@@ -2909,7 +3138,7 @@
         <v>0.6</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G10">
         <f t="shared" ref="G10:J10" si="3">G$7*$K4</f>
@@ -2940,7 +3169,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:J11" si="4">G$7*$K5</f>
@@ -2976,7 +3205,7 @@
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G13">
         <f>IF(G9&gt;0,(G3-G9)*(G3-G9)/G9,0)</f>
@@ -3348,28 +3577,28 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D1">
         <f>H9</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F1">
         <f>H18</f>
         <v>0.21875</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1">
         <f>H27</f>
         <v>0.375</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J1">
         <f>H36</f>
@@ -3381,7 +3610,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <f>D1-C16*F1-C25*H27-C34*J1</f>
@@ -3412,7 +3641,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2">
         <f>1-SUMSQ(E9:E12)</f>
@@ -3443,10 +3672,10 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3540,7 +3769,7 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E15" s="3">
         <f>1-SUMSQ(E18:E21)</f>
@@ -3575,10 +3804,10 @@
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -3672,7 +3901,7 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E24" s="2">
         <f>1-SUMSQ(E27:E30)</f>
@@ -3707,10 +3936,10 @@
         <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H26" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -3804,7 +4033,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E33" s="1">
         <f>1-SUMSQ(E36:E39)</f>
@@ -3839,10 +4068,10 @@
         <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H35" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -3941,7 +4170,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>0.5</v>
@@ -3950,15 +4179,15 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>

</xml_diff>